<commit_message>
Update to improve updateInvestmentAccount
</commit_message>
<xml_diff>
--- a/references/ACB Unit Tests.xlsx
+++ b/references/ACB Unit Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\pecuniary\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB85306-5569-46BE-AA19-11A3CA741304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FDC79F-7E05-464C-A6B7-C76A404A76F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28890" yWindow="3510" windowWidth="23655" windowHeight="17700" xr2:uid="{05D95A0F-6ADF-45BA-A18D-371BFBB70526}"/>
+    <workbookView xWindow="31095" yWindow="3855" windowWidth="25425" windowHeight="17310" xr2:uid="{05D95A0F-6ADF-45BA-A18D-371BFBB70526}"/>
   </bookViews>
   <sheets>
     <sheet name="ACB" sheetId="1" r:id="rId1"/>
@@ -42,10 +42,10 @@
     <t>bookValue</t>
   </si>
   <si>
-    <t>acb</t>
-  </si>
-  <si>
     <t>SELL</t>
+  </si>
+  <si>
+    <t>total</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <dimension ref="B2:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,10 +457,10 @@
         <v>3</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -509,7 +509,7 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1">
         <v>7</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>4</v>

</xml_diff>

<commit_message>
Improve updating investment account book and market values (#220)
* Update to improve updateInvestmentAccount

* Fix tests

* Fix tests

* Test

* Test

* Fix type

* Fix gitignore

* Refactor

* Update todo
</commit_message>
<xml_diff>
--- a/references/ACB Unit Tests.xlsx
+++ b/references/ACB Unit Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\pecuniary\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB85306-5569-46BE-AA19-11A3CA741304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FDC79F-7E05-464C-A6B7-C76A404A76F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28890" yWindow="3510" windowWidth="23655" windowHeight="17700" xr2:uid="{05D95A0F-6ADF-45BA-A18D-371BFBB70526}"/>
+    <workbookView xWindow="31095" yWindow="3855" windowWidth="25425" windowHeight="17310" xr2:uid="{05D95A0F-6ADF-45BA-A18D-371BFBB70526}"/>
   </bookViews>
   <sheets>
     <sheet name="ACB" sheetId="1" r:id="rId1"/>
@@ -42,10 +42,10 @@
     <t>bookValue</t>
   </si>
   <si>
-    <t>acb</t>
-  </si>
-  <si>
     <t>SELL</t>
+  </si>
+  <si>
+    <t>total</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <dimension ref="B2:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,10 +457,10 @@
         <v>3</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -509,7 +509,7 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1">
         <v>7</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>4</v>

</xml_diff>